<commit_message>
Updated code on timestamp:   16-05-2021
</commit_message>
<xml_diff>
--- a/Revision.xlsx
+++ b/Revision.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="475">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1620,46 +1620,10 @@
     <t xml:space="preserve">understand the traverse in backward direction </t>
   </si>
   <si>
-    <t>understand the traverse in backward direction</t>
-  </si>
-  <si>
-    <t>understand the traverse o  backward diliction</t>
-  </si>
-  <si>
-    <t>understand the traverse f  backward diktction</t>
-  </si>
-  <si>
-    <t>understand the traverse f  backward dimiction</t>
-  </si>
-  <si>
-    <t>understand the traverse or backward dimection</t>
-  </si>
-  <si>
-    <t>understand the traverse  L backward dimection</t>
-  </si>
-  <si>
-    <t>understand the traverse or backward direction</t>
-  </si>
-  <si>
-    <t>understand the traverse in backward diodction</t>
-  </si>
-  <si>
-    <t>understand the traverse n  backward dik ction</t>
-  </si>
-  <si>
-    <t>understand the traverse ev backward didiction</t>
-  </si>
-  <si>
-    <t>understand the traverse is backward diisction</t>
-  </si>
-  <si>
-    <t>understand the traverse  L backward difoction</t>
-  </si>
-  <si>
-    <t>understand the traverse wo backward diadction</t>
-  </si>
-  <si>
-    <t>understand the traverse f  backward diinction</t>
+    <t>addfirst, removefirst</t>
+  </si>
+  <si>
+    <t>addlast remove first</t>
   </si>
 </sst>
 </file>
@@ -6515,7 +6479,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6789,7 +6753,10 @@
         <v>34</v>
       </c>
       <c r="G15" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -6806,7 +6773,10 @@
         <v>34</v>
       </c>
       <c r="G16" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6823,7 +6793,7 @@
         <v>34</v>
       </c>
       <c r="G17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6840,7 +6810,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   16-05-2021 - 23:49:04.87
</commit_message>
<xml_diff>
--- a/Revision.xlsx
+++ b/Revision.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="478">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1624,6 +1624,16 @@
   </si>
   <si>
     <t>addlast remove first</t>
+  </si>
+  <si>
+    <t>use prev=null and curr =head
+traverse and change the link</t>
+  </si>
+  <si>
+    <t>slow =2 * fast</t>
+  </si>
+  <si>
+    <t>move fast k times and then move slow and fast together</t>
   </si>
 </sst>
 </file>
@@ -6479,7 +6489,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H13" sqref="H13:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6716,7 +6726,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>472</v>
@@ -6736,7 +6746,10 @@
         <v>34</v>
       </c>
       <c r="G14" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6755,7 +6768,7 @@
       <c r="G15" s="5">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="18" t="s">
         <v>473</v>
       </c>
     </row>
@@ -6775,11 +6788,11 @@
       <c r="G16" s="5">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="18" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <v>13</v>
       </c>
@@ -6795,8 +6808,11 @@
       <c r="G17" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="18" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="30">
         <v>14</v>
       </c>
@@ -6812,8 +6828,11 @@
       <c r="G18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="18" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>15</v>
       </c>
@@ -6830,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>16</v>
       </c>
@@ -6847,7 +6866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>17</v>
       </c>
@@ -6858,7 +6877,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>18</v>
       </c>
@@ -6869,7 +6888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>19</v>
       </c>
@@ -6880,7 +6899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>20</v>
       </c>
@@ -6891,7 +6910,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>21</v>
       </c>
@@ -6902,7 +6921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30">
         <v>22</v>
       </c>
@@ -6913,7 +6932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="30">
         <v>23</v>
       </c>
@@ -6924,7 +6943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>24</v>
       </c>
@@ -6935,7 +6954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   16-05-2021 - 23:51:06.54
</commit_message>
<xml_diff>
--- a/Revision.xlsx
+++ b/Revision.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Leet" sheetId="13" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="479">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1634,6 +1634,9 @@
   </si>
   <si>
     <t>move fast k times and then move slow and fast together</t>
+  </si>
+  <si>
+    <t>Pep_Combination_Sum | TSP1+TSP2 : Test1 Question | Contests | HackerRank</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1923,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2163,6 +2166,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -3344,10 +3350,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4293,6 +4299,17 @@
       </c>
       <c r="K36" s="16" t="s">
         <v>458</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>34</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="D37" s="87" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4316,9 +4333,10 @@
     <hyperlink ref="K36" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/HackerRankRecursiveDigit_sum.java"/>
     <hyperlink ref="K35" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.java"/>
     <hyperlink ref="D35" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.txt"/>
+    <hyperlink ref="D37" r:id="rId20" display="https://www.hackerrank.com/contests/tsp1tsp2-test1/challenges/pep-combination-sum/problem"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -4327,7 +4345,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6488,8 +6506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>